<commit_message>
Fix filter button shadows, update card backgrounds to white, add logout confirmation, update date inputs to dd-mm-yyyy format, import Rich Dad transactions
</commit_message>
<xml_diff>
--- a/rich_dad_transactions_from_pdf.xlsx
+++ b/rich_dad_transactions_from_pdf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chinmaya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFDA710-A0CA-42F6-BAED-40D9662A76DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A132AF24-A83F-435D-961C-E01CD2D97BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4116" yWindow="2220" windowWidth="17172" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Added by</t>
   </si>
   <si>
-    <t>2025-10-30</t>
-  </si>
-  <si>
     <t>Expense</t>
   </si>
   <si>
@@ -54,27 +51,18 @@
     <t>Chinmaya Kapopara</t>
   </si>
   <si>
-    <t>2025-10-27</t>
-  </si>
-  <si>
     <t>CRK</t>
   </si>
   <si>
     <t>Aps. Dahej rtn by JBk</t>
   </si>
   <si>
-    <t>2025-10-18</t>
-  </si>
-  <si>
     <t>RCK</t>
   </si>
   <si>
     <t>Reports for Children</t>
   </si>
   <si>
-    <t>2025-10-17</t>
-  </si>
-  <si>
     <t>Income</t>
   </si>
   <si>
@@ -84,36 +72,21 @@
     <t>Dahej Na Exp Share to GR Sheladiya as 10%</t>
   </si>
   <si>
-    <t>2025-10-15</t>
-  </si>
-  <si>
     <t>JRK milk bill</t>
   </si>
   <si>
-    <t>2025-10-14</t>
-  </si>
-  <si>
     <t>JRK</t>
   </si>
   <si>
-    <t>2025-10-12</t>
-  </si>
-  <si>
     <t>Jbk bombay</t>
   </si>
   <si>
-    <t>2025-10-11</t>
-  </si>
-  <si>
     <t>Opening Bal CB + Locker</t>
   </si>
   <si>
     <t>TL balance</t>
   </si>
   <si>
-    <t>2025-11-29</t>
-  </si>
-  <si>
     <t>ICICI Deposit - Hansaben</t>
   </si>
   <si>
@@ -123,90 +96,36 @@
     <t>ICICI Deposit - GLK</t>
   </si>
   <si>
-    <t>2025-11-24</t>
-  </si>
-  <si>
-    <t>2025-11-22</t>
-  </si>
-  <si>
     <t>Gir Gadhada Ent JBK</t>
   </si>
   <si>
-    <t>2025-11-15</t>
-  </si>
-  <si>
     <t>Gofalo</t>
   </si>
   <si>
-    <t>2025-11-11</t>
-  </si>
-  <si>
     <t>Mahendra dindoli salary</t>
   </si>
   <si>
-    <t>2025-11-09</t>
-  </si>
-  <si>
     <t>A - 803 Uchak Ent By JBK</t>
   </si>
   <si>
-    <t>2025-11-06</t>
-  </si>
-  <si>
-    <t>2025-11-05</t>
-  </si>
-  <si>
     <t>SPK Rajubhai Return Int</t>
   </si>
   <si>
-    <t>2025-11-01</t>
-  </si>
-  <si>
-    <t>2025-12-31</t>
-  </si>
-  <si>
     <t>Gir Gadhada - BGK Ent JBK</t>
   </si>
   <si>
-    <t>2025-12-30</t>
-  </si>
-  <si>
     <t>SPK to Paragbhai Ent JBK</t>
   </si>
   <si>
-    <t>2025-12-25</t>
-  </si>
-  <si>
-    <t>2025-12-15</t>
-  </si>
-  <si>
-    <t>2025-12-13</t>
-  </si>
-  <si>
-    <t>2025-12-11</t>
-  </si>
-  <si>
     <t>Mahendra dindoli 82/04 stamp reg by CRK</t>
   </si>
   <si>
-    <t>2025-12-09</t>
-  </si>
-  <si>
     <t>Mahendra - Dindoli (82-104)</t>
   </si>
   <si>
-    <t>2025-12-08</t>
-  </si>
-  <si>
-    <t>2025-12-07</t>
-  </si>
-  <si>
     <t>Vidhi Ladva Hare Krushna - RGK</t>
   </si>
   <si>
-    <t>2025-12-06</t>
-  </si>
-  <si>
     <t>KRC Bracelet</t>
   </si>
   <si>
@@ -216,18 +135,9 @@
     <t>APS</t>
   </si>
   <si>
-    <t>2025-12-04</t>
-  </si>
-  <si>
-    <t>2025-12-01</t>
-  </si>
-  <si>
     <t>Baa Hospital - RCK</t>
   </si>
   <si>
-    <t>2026-01-13</t>
-  </si>
-  <si>
     <t>JBK</t>
   </si>
   <si>
@@ -237,31 +147,16 @@
     <t>BGK gadhada krishna park</t>
   </si>
   <si>
-    <t>2026-01-09</t>
-  </si>
-  <si>
     <t>R c boda int up to 31.12.25</t>
   </si>
   <si>
-    <t>2026-01-08</t>
-  </si>
-  <si>
-    <t>2026-01-07</t>
-  </si>
-  <si>
     <t>Anandbhai fee</t>
   </si>
   <si>
-    <t>2026-01-05</t>
-  </si>
-  <si>
     <t>Mahendra Dindoli brokerage</t>
   </si>
   <si>
     <t>Gunjanbhai - SID</t>
-  </si>
-  <si>
-    <t>2026-01-02</t>
   </si>
   <si>
     <t>IDFC Deposit - Nirva</t>
@@ -339,11 +234,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,12 +545,14 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -675,1057 +573,1057 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="2">
+        <v>45960</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>-220</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45957</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>-200</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2">
+        <v>45957</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
       <c r="D4">
         <v>-2000</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
+      <c r="A5" s="2">
+        <v>45948</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>-150</v>
       </c>
       <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45948</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
       <c r="D6">
         <v>-150</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="2">
+        <v>45948</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>-92</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
+      <c r="A8" s="2">
+        <v>45947</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>5000</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="A9" s="2">
+        <v>45947</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>-556</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>19</v>
+      <c r="A10" s="2">
+        <v>45945</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>-600</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
+      <c r="A11" s="2">
+        <v>45944</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>-300</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
+      <c r="A12" s="2">
+        <v>45942</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>-500</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
+      <c r="A13" s="2">
+        <v>45941</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>69675</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
+      <c r="A14" s="2">
+        <v>45941</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>-65000</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
+      <c r="A15" s="2">
+        <v>45990</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>-1000</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
+      <c r="A16" s="2">
+        <v>45990</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>-1000</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>28</v>
+      <c r="A17" s="2">
+        <v>45990</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>-1000</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>32</v>
+      <c r="A18" s="2">
+        <v>45985</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>-400</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>33</v>
+      <c r="A19" s="2">
+        <v>45983</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>23000</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>35</v>
+      <c r="A20" s="2">
+        <v>45976</v>
       </c>
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
       </c>
       <c r="D20">
         <v>-100</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>35</v>
+      <c r="A21" s="2">
+        <v>45976</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D21">
         <v>-695</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>37</v>
+      <c r="A22" s="2">
+        <v>45972</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D22">
         <v>-200</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>39</v>
+      <c r="A23" s="2">
+        <v>45970</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D23">
         <v>-1000</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>39</v>
+      <c r="A24" s="2">
+        <v>45970</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>-2444</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>41</v>
+      <c r="A25" s="2">
+        <v>45967</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D25">
         <v>-625</v>
       </c>
       <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45967</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
       </c>
       <c r="D26">
         <v>-375</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>42</v>
+      <c r="A27" s="2">
+        <v>45966</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>1000</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>44</v>
+      <c r="A28" s="2">
+        <v>45962</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D28">
         <v>10000</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>45</v>
+      <c r="A29" s="2">
+        <v>46022</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="D29">
         <v>-350</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>45</v>
+      <c r="A30" s="2">
+        <v>46022</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="D30">
         <v>-400</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>45</v>
+      <c r="A31" s="2">
+        <v>46022</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="D31">
         <v>-500</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>45</v>
+      <c r="A32" s="2">
+        <v>46022</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="D32">
         <v>-400</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>45</v>
+      <c r="A33" s="2">
+        <v>46022</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D33">
         <v>-500</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>45</v>
+      <c r="A34" s="2">
+        <v>46022</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>5000</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>47</v>
+      <c r="A35" s="2">
+        <v>46021</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D35">
         <v>-10000</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>49</v>
+      <c r="A36" s="2">
+        <v>46016</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>-500</v>
       </c>
       <c r="E36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>46006</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
       </c>
       <c r="D37">
         <v>-500</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>51</v>
+      <c r="A38" s="2">
+        <v>46004</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D38">
         <v>-500</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>52</v>
+      <c r="A39" s="2">
+        <v>46002</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D39">
         <v>-985</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>54</v>
+      <c r="A40" s="2">
+        <v>46000</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D40">
         <v>-538</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>56</v>
+      <c r="A41" s="2">
+        <v>45999</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D41">
         <v>-85</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>57</v>
+      <c r="A42" s="2">
+        <v>45998</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D42">
         <v>-900</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>59</v>
+      <c r="A43" s="2">
+        <v>45997</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="D43">
         <v>-850</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>59</v>
+      <c r="A44" s="2">
+        <v>45997</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="D44">
         <v>750</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>59</v>
+      <c r="A45" s="2">
+        <v>45997</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D45">
         <v>-1000</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>59</v>
+      <c r="A46" s="2">
+        <v>45997</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="D46">
         <v>-3500</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>63</v>
+      <c r="A47" s="2">
+        <v>45995</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D47">
         <v>-300</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>64</v>
+      <c r="A48" s="2">
+        <v>45992</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D48">
         <v>-200</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>66</v>
+      <c r="A49" s="2">
+        <v>46035</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="D49">
         <v>-1000</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>66</v>
+      <c r="A50" s="2">
+        <v>46035</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D50">
         <v>-10000</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>66</v>
+      <c r="A51" s="2">
+        <v>46035</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D51">
         <v>4000</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>70</v>
+      <c r="A52" s="2">
+        <v>46031</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D52">
         <v>1750</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>72</v>
+      <c r="A53" s="2">
+        <v>46030</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D53">
         <v>-480</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>73</v>
+      <c r="A54" s="2">
+        <v>46029</v>
       </c>
       <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
         <v>6</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
       </c>
       <c r="D54">
         <v>-60</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>73</v>
+      <c r="A55" s="2">
+        <v>46029</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D55">
         <v>-440</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>75</v>
+      <c r="A56" s="2">
+        <v>46027</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D56">
         <v>-520</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>75</v>
+      <c r="A57" s="2">
+        <v>46027</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>75</v>
+      <c r="A58" s="2">
+        <v>46027</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="D58">
         <v>20000</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>78</v>
+      <c r="A59" s="2">
+        <v>46024</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="D59">
         <v>-2000</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>78</v>
+      <c r="A60" s="2">
+        <v>46024</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D60">
         <v>-1000</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>78</v>
+      <c r="A61" s="2">
+        <v>46024</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D61">
         <v>-1000</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>78</v>
+      <c r="A62" s="2">
+        <v>46024</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D62">
         <v>-1000</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>78</v>
+      <c r="A63" s="2">
+        <v>46024</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D63">
         <v>-1000</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>